<commit_message>
Add README to sheep folder to explain contents of test-data files.
</commit_message>
<xml_diff>
--- a/sims/src/observations/sheep/aerial-population-total-count-recruitment-composition/2.1/test-data/EastKootenay_Sheep_Aerial_Total_Count_2.0.xlsx
+++ b/sims/src/observations/sheep/aerial-population-total-count-recruitment-composition/2.1/test-data/EastKootenay_Sheep_Aerial_Total_Count_2.0.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69894F0E-C32A-4D63-8FE2-CC792E25FEF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83775DC-5DA2-4CB9-AE8F-1532C6CDF57E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="648" xr2:uid="{EA928297-87AF-4A2F-92BD-649BD8B345BB}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1693" uniqueCount="538">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1685" uniqueCount="537">
   <si>
     <t>Date</t>
   </si>
@@ -1169,9 +1169,6 @@
   </si>
   <si>
     <t>Columbia Lake East</t>
-  </si>
-  <si>
-    <t>Sharktooth</t>
   </si>
   <si>
     <t>Elk Valley West</t>
@@ -2198,47 +2195,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="3" xr:uid="{B247C600-A4F1-4276-B03B-332EB57CCBE3}"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2609,10 +2566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9934F4F-97FC-4CFD-8FF0-86937AF9AE11}">
-  <dimension ref="A1:AJ288"/>
+  <dimension ref="A1:AJ287"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2798,16 +2755,16 @@
         <v>0</v>
       </c>
       <c r="R2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="S2" s="39" t="s">
         <v>192</v>
       </c>
       <c r="T2" t="s">
+        <v>385</v>
+      </c>
+      <c r="U2" s="70" t="s">
         <v>386</v>
-      </c>
-      <c r="U2" s="70" t="s">
-        <v>387</v>
       </c>
       <c r="V2" s="70"/>
       <c r="W2" s="70"/>
@@ -2815,13 +2772,13 @@
         <v>-12</v>
       </c>
       <c r="Y2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="Z2">
         <v>0</v>
       </c>
       <c r="AA2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AB2" s="38"/>
       <c r="AC2" s="38"/>
@@ -2830,7 +2787,7 @@
       <c r="AF2" s="38"/>
       <c r="AG2" s="38"/>
       <c r="AH2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="AI2" s="38"/>
       <c r="AJ2" s="38"/>
@@ -2868,32 +2825,32 @@
         <v>0.67847222222222225</v>
       </c>
       <c r="N3" s="65">
-        <f t="shared" ref="N3:N11" si="0">(G3-F3)+(I3-H3)+(K3-J3)+(M3-L3)</f>
+        <f t="shared" ref="N3:N10" si="0">(G3-F3)+(I3-H3)+(K3-J3)+(M3-L3)</f>
         <v>4.7222222222222165E-2</v>
       </c>
       <c r="O3" s="66">
-        <f t="shared" ref="O3:O11" si="1">INT(N3)*24+HOUR(N3)+ROUND(MINUTE(N3)/60,2)</f>
+        <f t="shared" ref="O3:O10" si="1">INT(N3)*24+HOUR(N3)+ROUND(MINUTE(N3)/60,2)</f>
         <v>1.1299999999999999</v>
       </c>
       <c r="P3" s="67">
-        <f t="shared" ref="P3:P11" si="2">O3*60</f>
+        <f t="shared" ref="P3:P10" si="2">O3*60</f>
         <v>67.8</v>
       </c>
       <c r="Q3" s="66">
-        <f t="shared" ref="Q3:Q11" si="3">IF(D3&gt;0, D3/P3,0)</f>
+        <f t="shared" ref="Q3:Q10" si="3">IF(D3&gt;0, D3/P3,0)</f>
         <v>0</v>
       </c>
       <c r="R3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="S3" s="39" t="s">
         <v>192</v>
       </c>
       <c r="T3" t="s">
+        <v>385</v>
+      </c>
+      <c r="U3" s="70" t="s">
         <v>386</v>
-      </c>
-      <c r="U3" s="70" t="s">
-        <v>387</v>
       </c>
       <c r="V3" s="70"/>
       <c r="W3" s="70"/>
@@ -2901,13 +2858,13 @@
         <v>-10</v>
       </c>
       <c r="Y3" s="72" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="Z3">
         <v>90</v>
       </c>
       <c r="AA3" s="72" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AB3" s="38"/>
       <c r="AC3" s="38"/>
@@ -2964,16 +2921,16 @@
         <v>0</v>
       </c>
       <c r="R4" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="S4" s="39" t="s">
         <v>192</v>
       </c>
       <c r="T4" t="s">
+        <v>385</v>
+      </c>
+      <c r="U4" s="70" t="s">
         <v>386</v>
-      </c>
-      <c r="U4" s="70" t="s">
-        <v>387</v>
       </c>
       <c r="V4" s="70"/>
       <c r="W4" s="70"/>
@@ -2981,13 +2938,13 @@
         <v>-10</v>
       </c>
       <c r="Y4" s="72" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="Z4">
         <v>30</v>
       </c>
       <c r="AA4" s="72" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AB4" s="38"/>
       <c r="AC4" s="38"/>
@@ -3007,67 +2964,62 @@
         <v>379</v>
       </c>
       <c r="C5" s="61">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D5" s="35"/>
       <c r="E5" s="63">
-        <v>43494</v>
+        <v>43501</v>
       </c>
       <c r="F5" s="64">
-        <v>0.41250000000000003</v>
+        <v>0.4861111111111111</v>
       </c>
       <c r="G5" s="64">
-        <v>0.50694444444444442</v>
-      </c>
-      <c r="H5" s="64">
-        <v>0.54236111111111118</v>
-      </c>
-      <c r="I5" s="64">
-        <v>0.59027777777777779</v>
-      </c>
+        <v>0.58888888888888891</v>
+      </c>
+      <c r="H5"/>
+      <c r="I5"/>
       <c r="J5"/>
       <c r="K5"/>
       <c r="N5" s="65">
         <f t="shared" si="0"/>
-        <v>0.14236111111111099</v>
+        <v>0.1027777777777778</v>
       </c>
       <c r="O5" s="66">
         <f t="shared" si="1"/>
-        <v>3.42</v>
+        <v>2.4699999999999998</v>
       </c>
       <c r="P5" s="67">
         <f t="shared" si="2"/>
-        <v>205.2</v>
+        <v>148.19999999999999</v>
       </c>
       <c r="Q5" s="66">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R5" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="S5" s="39" t="s">
         <v>192</v>
       </c>
       <c r="T5" t="s">
+        <v>388</v>
+      </c>
+      <c r="U5" s="71" t="s">
         <v>389</v>
       </c>
-      <c r="U5" s="70" t="s">
-        <v>387</v>
-      </c>
       <c r="V5" s="70"/>
-      <c r="W5" s="70"/>
       <c r="X5">
-        <v>-18</v>
+        <v>-9</v>
       </c>
       <c r="Y5" s="72" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="Z5">
         <v>0</v>
       </c>
       <c r="AA5" s="72" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AB5" s="38"/>
       <c r="AC5" s="38"/>
@@ -3086,18 +3038,18 @@
       <c r="B6" t="s">
         <v>380</v>
       </c>
-      <c r="C6" s="61">
-        <v>4</v>
+      <c r="C6" s="62">
+        <v>3</v>
       </c>
       <c r="D6" s="35"/>
       <c r="E6" s="63">
-        <v>43501</v>
+        <v>43502</v>
       </c>
       <c r="F6" s="64">
-        <v>0.4861111111111111</v>
+        <v>0.39097222222222222</v>
       </c>
       <c r="G6" s="64">
-        <v>0.58888888888888891</v>
+        <v>0.50555555555555554</v>
       </c>
       <c r="H6"/>
       <c r="I6"/>
@@ -3105,44 +3057,45 @@
       <c r="K6"/>
       <c r="N6" s="65">
         <f t="shared" si="0"/>
-        <v>0.1027777777777778</v>
+        <v>0.11458333333333331</v>
       </c>
       <c r="O6" s="66">
         <f t="shared" si="1"/>
-        <v>2.4699999999999998</v>
+        <v>2.75</v>
       </c>
       <c r="P6" s="67">
         <f t="shared" si="2"/>
-        <v>148.19999999999999</v>
+        <v>165</v>
       </c>
       <c r="Q6" s="66">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R6" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="S6" s="39" t="s">
         <v>192</v>
       </c>
       <c r="T6" t="s">
+        <v>390</v>
+      </c>
+      <c r="U6" s="71" t="s">
         <v>389</v>
       </c>
-      <c r="U6" s="71" t="s">
-        <v>390</v>
-      </c>
       <c r="V6" s="70"/>
+      <c r="W6"/>
       <c r="X6">
-        <v>-9</v>
+        <v>-19</v>
       </c>
       <c r="Y6" s="72" t="s">
+        <v>391</v>
+      </c>
+      <c r="Z6">
+        <v>100</v>
+      </c>
+      <c r="AA6" s="72" t="s">
         <v>392</v>
-      </c>
-      <c r="Z6">
-        <v>0</v>
-      </c>
-      <c r="AA6" s="72" t="s">
-        <v>393</v>
       </c>
       <c r="AB6" s="38"/>
       <c r="AC6" s="38"/>
@@ -3162,17 +3115,17 @@
         <v>381</v>
       </c>
       <c r="C7" s="62">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D7" s="35"/>
       <c r="E7" s="63">
-        <v>43502</v>
+        <v>43517</v>
       </c>
       <c r="F7" s="64">
-        <v>0.39097222222222222</v>
+        <v>0.375</v>
       </c>
       <c r="G7" s="64">
-        <v>0.50555555555555554</v>
+        <v>0.4513888888888889</v>
       </c>
       <c r="H7"/>
       <c r="I7"/>
@@ -3180,44 +3133,43 @@
       <c r="K7"/>
       <c r="N7" s="65">
         <f t="shared" si="0"/>
-        <v>0.11458333333333331</v>
+        <v>7.6388888888888895E-2</v>
       </c>
       <c r="O7" s="66">
         <f t="shared" si="1"/>
-        <v>2.75</v>
+        <v>1.83</v>
       </c>
       <c r="P7" s="67">
         <f t="shared" si="2"/>
-        <v>165</v>
+        <v>109.80000000000001</v>
       </c>
       <c r="Q7" s="66">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R7" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="S7" s="39" t="s">
         <v>192</v>
       </c>
       <c r="T7" t="s">
+        <v>390</v>
+      </c>
+      <c r="U7" s="71" t="s">
+        <v>389</v>
+      </c>
+      <c r="V7" s="70"/>
+      <c r="X7">
+        <v>-12</v>
+      </c>
+      <c r="Y7" t="s">
         <v>391</v>
-      </c>
-      <c r="U7" s="71" t="s">
-        <v>390</v>
-      </c>
-      <c r="V7" s="70"/>
-      <c r="W7"/>
-      <c r="X7">
-        <v>-19</v>
-      </c>
-      <c r="Y7" s="72" t="s">
-        <v>392</v>
       </c>
       <c r="Z7">
         <v>100</v>
       </c>
-      <c r="AA7" s="72" t="s">
+      <c r="AA7" t="s">
         <v>393</v>
       </c>
       <c r="AB7" s="38"/>
@@ -3238,17 +3190,17 @@
         <v>382</v>
       </c>
       <c r="C8" s="62">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D8" s="35"/>
       <c r="E8" s="63">
-        <v>43517</v>
+        <v>43523</v>
       </c>
       <c r="F8" s="64">
-        <v>0.375</v>
+        <v>0.39930555555555558</v>
       </c>
       <c r="G8" s="64">
-        <v>0.4513888888888889</v>
+        <v>0.5</v>
       </c>
       <c r="H8"/>
       <c r="I8"/>
@@ -3256,44 +3208,44 @@
       <c r="K8"/>
       <c r="N8" s="65">
         <f t="shared" si="0"/>
-        <v>7.6388888888888895E-2</v>
+        <v>0.10069444444444442</v>
       </c>
       <c r="O8" s="66">
         <f t="shared" si="1"/>
-        <v>1.83</v>
+        <v>2.42</v>
       </c>
       <c r="P8" s="67">
         <f t="shared" si="2"/>
-        <v>109.80000000000001</v>
+        <v>145.19999999999999</v>
       </c>
       <c r="Q8" s="66">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R8" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="S8" s="39" t="s">
         <v>192</v>
       </c>
       <c r="T8" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="U8" s="71" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="V8" s="70"/>
       <c r="X8">
         <v>-12</v>
       </c>
       <c r="Y8" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="Z8">
         <v>100</v>
       </c>
       <c r="AA8" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="AB8" s="38"/>
       <c r="AC8" s="38"/>
@@ -3313,17 +3265,17 @@
         <v>383</v>
       </c>
       <c r="C9" s="62">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D9" s="35"/>
       <c r="E9" s="63">
         <v>43523</v>
       </c>
       <c r="F9" s="64">
-        <v>0.39930555555555558</v>
+        <v>0.53263888888888888</v>
       </c>
       <c r="G9" s="64">
-        <v>0.5</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="H9"/>
       <c r="I9"/>
@@ -3331,44 +3283,44 @@
       <c r="K9"/>
       <c r="N9" s="65">
         <f t="shared" si="0"/>
-        <v>0.10069444444444442</v>
+        <v>0.11319444444444449</v>
       </c>
       <c r="O9" s="66">
         <f t="shared" si="1"/>
-        <v>2.42</v>
+        <v>2.7199999999999998</v>
       </c>
       <c r="P9" s="67">
         <f t="shared" si="2"/>
-        <v>145.19999999999999</v>
+        <v>163.19999999999999</v>
       </c>
       <c r="Q9" s="66">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R9" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="S9" s="39" t="s">
         <v>192</v>
       </c>
       <c r="T9" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="U9" s="71" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="V9" s="70"/>
       <c r="X9">
         <v>-12</v>
       </c>
       <c r="Y9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="Z9">
         <v>100</v>
       </c>
       <c r="AA9" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="AB9" s="38"/>
       <c r="AC9" s="38"/>
@@ -3385,65 +3337,69 @@
         <v>375</v>
       </c>
       <c r="B10" t="s">
-        <v>384</v>
-      </c>
-      <c r="C10" s="62">
-        <v>5</v>
+        <v>378</v>
+      </c>
+      <c r="C10" s="3">
+        <v>8</v>
       </c>
       <c r="D10" s="35"/>
       <c r="E10" s="63">
         <v>43523</v>
       </c>
       <c r="F10" s="64">
-        <v>0.53263888888888888</v>
+        <v>0.42499999999999999</v>
       </c>
       <c r="G10" s="64">
-        <v>0.64583333333333337</v>
-      </c>
-      <c r="H10"/>
-      <c r="I10"/>
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="H10" s="64">
+        <v>0.52013888888888882</v>
+      </c>
+      <c r="I10" s="64">
+        <v>0.57986111111111105</v>
+      </c>
       <c r="J10"/>
       <c r="K10"/>
       <c r="N10" s="65">
         <f t="shared" si="0"/>
-        <v>0.11319444444444449</v>
+        <v>0.14513888888888887</v>
       </c>
       <c r="O10" s="66">
         <f t="shared" si="1"/>
-        <v>2.7199999999999998</v>
+        <v>3.48</v>
       </c>
       <c r="P10" s="67">
         <f t="shared" si="2"/>
-        <v>163.19999999999999</v>
+        <v>208.8</v>
       </c>
       <c r="Q10" s="66">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R10" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="S10" s="39" t="s">
         <v>192</v>
       </c>
       <c r="T10" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="U10" s="71" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="V10" s="70"/>
       <c r="X10">
-        <v>-12</v>
-      </c>
-      <c r="Y10" t="s">
-        <v>392</v>
+        <v>-11</v>
+      </c>
+      <c r="Y10" s="72" t="s">
+        <v>391</v>
       </c>
       <c r="Z10">
         <v>100</v>
       </c>
       <c r="AA10" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="AB10" s="38"/>
       <c r="AC10" s="38"/>
@@ -3456,74 +3412,24 @@
       <c r="AJ10" s="38"/>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A11" s="59" t="s">
-        <v>375</v>
-      </c>
-      <c r="B11" t="s">
-        <v>378</v>
-      </c>
-      <c r="C11" s="3">
-        <v>8</v>
-      </c>
+      <c r="A11" s="32"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="34"/>
       <c r="D11" s="35"/>
-      <c r="E11" s="63">
-        <v>43523</v>
-      </c>
-      <c r="F11" s="64">
-        <v>0.42499999999999999</v>
-      </c>
-      <c r="G11" s="64">
-        <v>0.51041666666666663</v>
-      </c>
-      <c r="H11" s="64">
-        <v>0.52013888888888882</v>
-      </c>
-      <c r="I11" s="64">
-        <v>0.57986111111111105</v>
-      </c>
-      <c r="J11"/>
-      <c r="K11"/>
-      <c r="N11" s="65">
-        <f t="shared" si="0"/>
-        <v>0.14513888888888887</v>
-      </c>
-      <c r="O11" s="66">
-        <f t="shared" si="1"/>
-        <v>3.48</v>
-      </c>
-      <c r="P11" s="67">
-        <f t="shared" si="2"/>
-        <v>208.8</v>
-      </c>
-      <c r="Q11" s="66">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="R11" t="s">
-        <v>385</v>
-      </c>
-      <c r="S11" s="39" t="s">
-        <v>192</v>
-      </c>
-      <c r="T11" t="s">
-        <v>391</v>
-      </c>
-      <c r="U11" s="71" t="s">
-        <v>390</v>
-      </c>
-      <c r="V11" s="70"/>
-      <c r="X11">
-        <v>-11</v>
-      </c>
-      <c r="Y11" s="72" t="s">
-        <v>392</v>
-      </c>
-      <c r="Z11">
-        <v>100</v>
-      </c>
-      <c r="AA11" t="s">
-        <v>394</v>
-      </c>
+      <c r="N11" s="41"/>
+      <c r="O11" s="41"/>
+      <c r="P11" s="41"/>
+      <c r="Q11" s="41"/>
+      <c r="R11" s="35"/>
+      <c r="S11" s="39"/>
+      <c r="T11" s="38"/>
+      <c r="U11" s="38"/>
+      <c r="V11" s="38"/>
+      <c r="W11" s="38"/>
+      <c r="X11" s="32"/>
+      <c r="Y11" s="38"/>
+      <c r="Z11" s="38"/>
+      <c r="AA11" s="38"/>
       <c r="AB11" s="38"/>
       <c r="AC11" s="38"/>
       <c r="AD11" s="38"/>
@@ -4380,10 +4286,10 @@
       <c r="B41" s="33"/>
       <c r="C41" s="34"/>
       <c r="D41" s="35"/>
-      <c r="N41" s="41"/>
-      <c r="O41" s="41"/>
-      <c r="P41" s="41"/>
-      <c r="Q41" s="41"/>
+      <c r="N41" s="42"/>
+      <c r="O41" s="42"/>
+      <c r="P41" s="42"/>
+      <c r="Q41" s="42"/>
       <c r="R41" s="35"/>
       <c r="S41" s="39"/>
       <c r="T41" s="38"/>
@@ -5163,10 +5069,10 @@
       <c r="B68" s="33"/>
       <c r="C68" s="34"/>
       <c r="D68" s="35"/>
-      <c r="N68" s="42"/>
-      <c r="O68" s="42"/>
-      <c r="P68" s="42"/>
-      <c r="Q68" s="42"/>
+      <c r="N68" s="41"/>
+      <c r="O68" s="41"/>
+      <c r="P68" s="41"/>
+      <c r="Q68" s="41"/>
       <c r="R68" s="35"/>
       <c r="S68" s="39"/>
       <c r="T68" s="38"/>
@@ -5598,10 +5504,10 @@
       <c r="B83" s="33"/>
       <c r="C83" s="34"/>
       <c r="D83" s="35"/>
-      <c r="N83" s="41"/>
-      <c r="O83" s="41"/>
-      <c r="P83" s="41"/>
-      <c r="Q83" s="41"/>
+      <c r="N83" s="42"/>
+      <c r="O83" s="42"/>
+      <c r="P83" s="42"/>
+      <c r="Q83" s="42"/>
       <c r="R83" s="35"/>
       <c r="S83" s="39"/>
       <c r="T83" s="38"/>
@@ -5888,10 +5794,10 @@
       <c r="B93" s="33"/>
       <c r="C93" s="34"/>
       <c r="D93" s="35"/>
-      <c r="N93" s="42"/>
-      <c r="O93" s="42"/>
-      <c r="P93" s="42"/>
-      <c r="Q93" s="42"/>
+      <c r="N93" s="41"/>
+      <c r="O93" s="41"/>
+      <c r="P93" s="41"/>
+      <c r="Q93" s="41"/>
       <c r="R93" s="35"/>
       <c r="S93" s="39"/>
       <c r="T93" s="38"/>
@@ -6087,33 +5993,27 @@
       <c r="AJ99" s="38"/>
     </row>
     <row r="100" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A100" s="32"/>
-      <c r="B100" s="33"/>
-      <c r="C100" s="34"/>
+      <c r="C100" s="43"/>
       <c r="D100" s="35"/>
+      <c r="E100" s="44"/>
+      <c r="F100" s="45"/>
+      <c r="G100" s="45"/>
+      <c r="H100" s="45"/>
+      <c r="I100" s="45"/>
+      <c r="J100" s="45"/>
+      <c r="K100" s="45"/>
+      <c r="L100" s="45"/>
+      <c r="M100" s="45"/>
       <c r="N100" s="41"/>
       <c r="O100" s="41"/>
       <c r="P100" s="41"/>
       <c r="Q100" s="41"/>
-      <c r="R100" s="35"/>
-      <c r="S100" s="39"/>
-      <c r="T100" s="38"/>
-      <c r="U100" s="38"/>
-      <c r="V100" s="38"/>
-      <c r="W100" s="38"/>
-      <c r="X100" s="32"/>
-      <c r="Y100" s="38"/>
-      <c r="Z100" s="38"/>
-      <c r="AA100" s="38"/>
-      <c r="AB100" s="38"/>
-      <c r="AC100" s="38"/>
-      <c r="AD100" s="38"/>
-      <c r="AE100" s="38"/>
-      <c r="AF100" s="38"/>
-      <c r="AG100" s="38"/>
-      <c r="AH100" s="38"/>
-      <c r="AI100" s="38"/>
-      <c r="AJ100" s="38"/>
+      <c r="R100" s="41"/>
+      <c r="S100" s="41"/>
+      <c r="T100" s="41"/>
+      <c r="U100" s="17"/>
+      <c r="V100" s="17"/>
+      <c r="W100" s="17"/>
     </row>
     <row r="101" spans="1:36" x14ac:dyDescent="0.25">
       <c r="C101" s="43"/>
@@ -6992,22 +6892,13 @@
     <row r="139" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C139" s="43"/>
       <c r="D139" s="35"/>
-      <c r="E139" s="44"/>
-      <c r="F139" s="45"/>
-      <c r="G139" s="45"/>
-      <c r="H139" s="45"/>
-      <c r="I139" s="45"/>
-      <c r="J139" s="45"/>
-      <c r="K139" s="45"/>
-      <c r="L139" s="45"/>
-      <c r="M139" s="45"/>
       <c r="N139" s="41"/>
       <c r="O139" s="41"/>
       <c r="P139" s="41"/>
       <c r="Q139" s="41"/>
-      <c r="R139" s="41"/>
-      <c r="S139" s="41"/>
-      <c r="T139" s="41"/>
+      <c r="R139" s="42"/>
+      <c r="S139" s="42"/>
+      <c r="T139" s="42"/>
       <c r="U139" s="17"/>
       <c r="V139" s="17"/>
       <c r="W139" s="17"/>
@@ -7377,15 +7268,24 @@
       <c r="W165" s="17"/>
     </row>
     <row r="166" spans="3:23" x14ac:dyDescent="0.25">
-      <c r="C166" s="43"/>
+      <c r="C166" s="46"/>
       <c r="D166" s="35"/>
+      <c r="E166" s="44"/>
+      <c r="F166" s="45"/>
+      <c r="G166" s="45"/>
+      <c r="H166" s="45"/>
+      <c r="I166" s="45"/>
+      <c r="J166" s="45"/>
+      <c r="K166" s="45"/>
+      <c r="L166" s="45"/>
+      <c r="M166" s="45"/>
       <c r="N166" s="41"/>
       <c r="O166" s="41"/>
       <c r="P166" s="41"/>
       <c r="Q166" s="41"/>
-      <c r="R166" s="42"/>
-      <c r="S166" s="42"/>
-      <c r="T166" s="42"/>
+      <c r="R166" s="41"/>
+      <c r="S166" s="41"/>
+      <c r="T166" s="41"/>
       <c r="U166" s="17"/>
       <c r="V166" s="17"/>
       <c r="W166" s="17"/>
@@ -7713,24 +7613,15 @@
       <c r="W180" s="17"/>
     </row>
     <row r="181" spans="3:23" x14ac:dyDescent="0.25">
-      <c r="C181" s="46"/>
+      <c r="C181" s="43"/>
       <c r="D181" s="35"/>
-      <c r="E181" s="44"/>
-      <c r="F181" s="45"/>
-      <c r="G181" s="45"/>
-      <c r="H181" s="45"/>
-      <c r="I181" s="45"/>
-      <c r="J181" s="45"/>
-      <c r="K181" s="45"/>
-      <c r="L181" s="45"/>
-      <c r="M181" s="45"/>
       <c r="N181" s="41"/>
       <c r="O181" s="41"/>
       <c r="P181" s="41"/>
       <c r="Q181" s="41"/>
-      <c r="R181" s="41"/>
-      <c r="S181" s="41"/>
-      <c r="T181" s="41"/>
+      <c r="R181" s="42"/>
+      <c r="S181" s="42"/>
+      <c r="T181" s="42"/>
       <c r="U181" s="17"/>
       <c r="V181" s="17"/>
       <c r="W181" s="17"/>
@@ -7836,10 +7727,10 @@
     <row r="189" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C189" s="43"/>
       <c r="D189" s="35"/>
-      <c r="N189" s="41"/>
-      <c r="O189" s="41"/>
-      <c r="P189" s="41"/>
-      <c r="Q189" s="41"/>
+      <c r="N189" s="47"/>
+      <c r="O189" s="47"/>
+      <c r="P189" s="47"/>
+      <c r="Q189" s="47"/>
       <c r="R189" s="42"/>
       <c r="S189" s="42"/>
       <c r="T189" s="42"/>
@@ -7850,10 +7741,6 @@
     <row r="190" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C190" s="43"/>
       <c r="D190" s="35"/>
-      <c r="N190" s="47"/>
-      <c r="O190" s="47"/>
-      <c r="P190" s="47"/>
-      <c r="Q190" s="47"/>
       <c r="R190" s="42"/>
       <c r="S190" s="42"/>
       <c r="T190" s="42"/>
@@ -7862,11 +7749,20 @@
       <c r="W190" s="17"/>
     </row>
     <row r="191" spans="3:23" x14ac:dyDescent="0.25">
-      <c r="C191" s="43"/>
+      <c r="C191" s="46"/>
       <c r="D191" s="35"/>
-      <c r="R191" s="42"/>
-      <c r="S191" s="42"/>
-      <c r="T191" s="42"/>
+      <c r="E191" s="44"/>
+      <c r="F191" s="45"/>
+      <c r="G191" s="45"/>
+      <c r="H191" s="45"/>
+      <c r="I191" s="45"/>
+      <c r="J191" s="45"/>
+      <c r="K191" s="45"/>
+      <c r="L191" s="45"/>
+      <c r="M191" s="45"/>
+      <c r="R191" s="41"/>
+      <c r="S191" s="41"/>
+      <c r="T191" s="41"/>
       <c r="U191" s="17"/>
       <c r="V191" s="17"/>
       <c r="W191" s="17"/>
@@ -8252,7 +8148,7 @@
       <c r="W211" s="17"/>
     </row>
     <row r="212" spans="3:23" x14ac:dyDescent="0.25">
-      <c r="C212" s="46"/>
+      <c r="C212" s="43"/>
       <c r="D212" s="35"/>
       <c r="E212" s="44"/>
       <c r="F212" s="45"/>
@@ -8575,7 +8471,7 @@
       <c r="W228" s="17"/>
     </row>
     <row r="229" spans="3:23" x14ac:dyDescent="0.25">
-      <c r="C229" s="43"/>
+      <c r="C229" s="46"/>
       <c r="D229" s="35"/>
       <c r="E229" s="44"/>
       <c r="F229" s="45"/>
@@ -9677,83 +9573,48 @@
       <c r="W286" s="17"/>
     </row>
     <row r="287" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="C287" s="46"/>
-      <c r="D287" s="35"/>
-      <c r="E287" s="44"/>
-      <c r="F287" s="45"/>
-      <c r="G287" s="45"/>
-      <c r="H287" s="45"/>
-      <c r="I287" s="45"/>
-      <c r="J287" s="45"/>
-      <c r="K287" s="45"/>
-      <c r="L287" s="45"/>
-      <c r="M287" s="45"/>
-      <c r="R287" s="41"/>
-      <c r="S287" s="41"/>
-      <c r="T287" s="41"/>
-      <c r="U287" s="17"/>
-      <c r="V287" s="17"/>
-      <c r="W287" s="17"/>
-    </row>
-    <row r="288" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A288" s="47"/>
-      <c r="B288" s="47"/>
-      <c r="C288" s="47"/>
-      <c r="D288" s="48"/>
-      <c r="E288" s="49"/>
-      <c r="F288" s="50"/>
-      <c r="G288" s="50"/>
-      <c r="H288" s="50"/>
-      <c r="I288" s="50"/>
-      <c r="J288" s="50"/>
-      <c r="K288" s="50"/>
-      <c r="L288" s="50"/>
-      <c r="M288" s="50"/>
-      <c r="R288" s="47"/>
-      <c r="S288" s="47"/>
-      <c r="T288" s="47"/>
-      <c r="U288" s="47"/>
-      <c r="V288" s="47"/>
-      <c r="W288" s="47"/>
+      <c r="A287" s="47"/>
+      <c r="B287" s="47"/>
+      <c r="C287" s="47"/>
+      <c r="D287" s="48"/>
+      <c r="E287" s="49"/>
+      <c r="F287" s="50"/>
+      <c r="G287" s="50"/>
+      <c r="H287" s="50"/>
+      <c r="I287" s="50"/>
+      <c r="J287" s="50"/>
+      <c r="K287" s="50"/>
+      <c r="L287" s="50"/>
+      <c r="M287" s="50"/>
+      <c r="R287" s="47"/>
+      <c r="S287" s="47"/>
+      <c r="T287" s="47"/>
+      <c r="U287" s="47"/>
+      <c r="V287" s="47"/>
+      <c r="W287" s="47"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D101:D287 R12:R100 T12:W100">
-    <cfRule type="cellIs" dxfId="9" priority="125" operator="equal">
+  <conditionalFormatting sqref="R11:R99 T11:W99 D2:D286 R2:S10">
+    <cfRule type="cellIs" dxfId="5" priority="125" operator="equal">
       <formula>"LD"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="126" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="126" operator="equal">
       <formula>"BV"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D100">
-    <cfRule type="cellIs" dxfId="7" priority="13" operator="equal">
+  <conditionalFormatting sqref="S11:S99">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>"LD"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
       <formula>"BV"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S12:S100">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+  <conditionalFormatting sqref="T2:W4 V7:V10 V6:W6 T6:U10 T5:V5">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"LD"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
-      <formula>"BV"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R2:R11 T2:W5 V8:V11 V7:W7 T7:U11 T6:V6">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
-      <formula>"LD"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
-      <formula>"BV"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S2:S11">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
-      <formula>"LD"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"BV"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9766,7 +9627,7 @@
           <x14:formula1>
             <xm:f>Picklist!$A$2:$A$18</xm:f>
           </x14:formula1>
-          <xm:sqref>S12:S100</xm:sqref>
+          <xm:sqref>S11:S99</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -9960,7 +9821,7 @@
       <c r="H2" s="52"/>
       <c r="I2" s="52"/>
       <c r="J2" s="38" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="K2" s="63">
         <v>43493</v>
@@ -10026,7 +9887,7 @@
       <c r="H3" s="52"/>
       <c r="I3" s="52"/>
       <c r="J3" s="38" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="K3" s="63">
         <v>43493</v>
@@ -10094,7 +9955,7 @@
       <c r="H4" s="52"/>
       <c r="I4" s="52"/>
       <c r="J4" s="38" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="K4" s="63">
         <v>43493</v>
@@ -10164,7 +10025,7 @@
       <c r="H5" s="52"/>
       <c r="I5" s="52"/>
       <c r="J5" s="38" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="K5" s="63">
         <v>43493</v>
@@ -10232,7 +10093,7 @@
       <c r="H6" s="52"/>
       <c r="I6" s="52"/>
       <c r="J6" s="38" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="K6" s="63">
         <v>43493</v>
@@ -10298,7 +10159,7 @@
       <c r="H7" s="52"/>
       <c r="I7" s="52"/>
       <c r="J7" s="38" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="K7" s="63">
         <v>43493</v>
@@ -10364,7 +10225,7 @@
       <c r="H8" s="52"/>
       <c r="I8" s="52"/>
       <c r="J8" s="38" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="K8" s="63">
         <v>43493</v>
@@ -10430,7 +10291,7 @@
       <c r="H9" s="52"/>
       <c r="I9" s="52"/>
       <c r="J9" s="38" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="K9" s="63">
         <v>43493</v>
@@ -10496,7 +10357,7 @@
       <c r="H10" s="52"/>
       <c r="I10" s="52"/>
       <c r="J10" s="38" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="K10" s="63">
         <v>43493</v>
@@ -10564,7 +10425,7 @@
       <c r="H11" s="52"/>
       <c r="I11" s="52"/>
       <c r="J11" s="38" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="K11" s="63">
         <v>43493</v>
@@ -10632,7 +10493,7 @@
       <c r="H12" s="52"/>
       <c r="I12" s="52"/>
       <c r="J12" s="38" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="K12" s="63">
         <v>43493</v>
@@ -10700,7 +10561,7 @@
       <c r="H13" s="52"/>
       <c r="I13" s="52"/>
       <c r="J13" s="38" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="K13" s="63">
         <v>43493</v>
@@ -10770,7 +10631,7 @@
       <c r="H14" s="52"/>
       <c r="I14" s="52"/>
       <c r="J14" s="38" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="K14" s="63">
         <v>43493</v>
@@ -10838,7 +10699,7 @@
       <c r="H15" s="52"/>
       <c r="I15" s="52"/>
       <c r="J15" s="38" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="K15" s="63">
         <v>43493</v>
@@ -10904,7 +10765,7 @@
       <c r="H16" s="52"/>
       <c r="I16" s="52"/>
       <c r="J16" s="38" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="K16" s="63">
         <v>43493</v>
@@ -10978,7 +10839,7 @@
       <c r="H17" s="52"/>
       <c r="I17" s="52"/>
       <c r="J17" s="38" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="K17" s="63">
         <v>43493</v>
@@ -11026,7 +10887,7 @@
         <v>375</v>
       </c>
       <c r="B18" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C18" s="61">
         <v>4</v>
@@ -11046,7 +10907,7 @@
       <c r="H18" s="52"/>
       <c r="I18" s="52"/>
       <c r="J18" s="38" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="K18" s="63">
         <v>43501</v>
@@ -11090,7 +10951,7 @@
         <v>375</v>
       </c>
       <c r="B19" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C19" s="61">
         <v>4</v>
@@ -11110,7 +10971,7 @@
       <c r="H19" s="52"/>
       <c r="I19" s="52"/>
       <c r="J19" s="38" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K19" s="63">
         <v>43501</v>
@@ -11156,7 +11017,7 @@
         <v>375</v>
       </c>
       <c r="B20" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C20" s="61">
         <v>4</v>
@@ -11176,7 +11037,7 @@
       <c r="H20" s="52"/>
       <c r="I20" s="52"/>
       <c r="J20" s="38" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="K20" s="63">
         <v>43501</v>
@@ -11228,7 +11089,7 @@
         <v>375</v>
       </c>
       <c r="B21" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C21" s="61">
         <v>4</v>
@@ -11248,7 +11109,7 @@
       <c r="H21" s="52"/>
       <c r="I21" s="52"/>
       <c r="J21" s="38" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="K21" s="63">
         <v>43501</v>
@@ -11294,7 +11155,7 @@
         <v>375</v>
       </c>
       <c r="B22" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C22" s="61">
         <v>4</v>
@@ -11314,7 +11175,7 @@
       <c r="H22" s="52"/>
       <c r="I22" s="52"/>
       <c r="J22" s="38" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="K22" s="63">
         <v>43501</v>
@@ -11362,7 +11223,7 @@
         <v>375</v>
       </c>
       <c r="B23" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C23" s="61">
         <v>4</v>
@@ -11382,7 +11243,7 @@
       <c r="H23" s="52"/>
       <c r="I23" s="52"/>
       <c r="J23" s="38" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="K23" s="63">
         <v>43501</v>
@@ -11426,7 +11287,7 @@
         <v>375</v>
       </c>
       <c r="B24" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C24" s="61">
         <v>4</v>
@@ -11446,7 +11307,7 @@
       <c r="H24" s="52"/>
       <c r="I24" s="52"/>
       <c r="J24" s="38" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="K24" s="63">
         <v>43501</v>
@@ -11494,7 +11355,7 @@
         <v>375</v>
       </c>
       <c r="B25" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C25" s="61">
         <v>4</v>
@@ -11514,7 +11375,7 @@
       <c r="H25" s="52"/>
       <c r="I25" s="52"/>
       <c r="J25" s="38" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="K25" s="63">
         <v>43501</v>
@@ -11568,7 +11429,7 @@
         <v>375</v>
       </c>
       <c r="B26" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C26" s="62">
         <v>3</v>
@@ -11588,7 +11449,7 @@
       <c r="H26" s="52"/>
       <c r="I26" s="52"/>
       <c r="J26" s="38" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="K26" s="63">
         <v>43501</v>
@@ -11632,7 +11493,7 @@
         <v>375</v>
       </c>
       <c r="B27" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C27" s="62">
         <v>3</v>
@@ -11652,7 +11513,7 @@
       <c r="H27" s="52"/>
       <c r="I27" s="52"/>
       <c r="J27" s="38" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="K27" s="63">
         <v>43501</v>
@@ -11696,7 +11557,7 @@
         <v>375</v>
       </c>
       <c r="B28" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C28" s="62">
         <v>3</v>
@@ -11716,7 +11577,7 @@
       <c r="H28" s="52"/>
       <c r="I28" s="52"/>
       <c r="J28" s="38" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="K28" s="63">
         <v>43501</v>
@@ -11762,7 +11623,7 @@
         <v>375</v>
       </c>
       <c r="B29" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C29" s="62">
         <v>3</v>
@@ -11782,7 +11643,7 @@
       <c r="H29" s="52"/>
       <c r="I29" s="52"/>
       <c r="J29" s="38" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="K29" s="63">
         <v>43501</v>
@@ -11826,7 +11687,7 @@
         <v>375</v>
       </c>
       <c r="B30" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C30" s="62">
         <v>3</v>
@@ -11846,7 +11707,7 @@
       <c r="H30" s="52"/>
       <c r="I30" s="52"/>
       <c r="J30" s="38" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="K30" s="63">
         <v>43502</v>
@@ -11894,7 +11755,7 @@
         <v>375</v>
       </c>
       <c r="B31" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C31" s="62">
         <v>3</v>
@@ -11914,7 +11775,7 @@
       <c r="H31" s="52"/>
       <c r="I31" s="52"/>
       <c r="J31" s="38" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="K31" s="63">
         <v>43502</v>
@@ -11966,7 +11827,7 @@
         <v>375</v>
       </c>
       <c r="B32" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C32" s="62">
         <v>3</v>
@@ -11986,7 +11847,7 @@
       <c r="H32" s="52"/>
       <c r="I32" s="52"/>
       <c r="J32" s="38" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="K32" s="63">
         <v>43502</v>
@@ -12032,7 +11893,7 @@
         <v>375</v>
       </c>
       <c r="B33" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C33" s="62">
         <v>3</v>
@@ -12052,7 +11913,7 @@
       <c r="H33" s="52"/>
       <c r="I33" s="52"/>
       <c r="J33" s="38" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="K33" s="63">
         <v>43502</v>
@@ -12096,7 +11957,7 @@
         <v>375</v>
       </c>
       <c r="B34" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C34" s="62">
         <v>3</v>
@@ -12116,7 +11977,7 @@
       <c r="H34" s="52"/>
       <c r="I34" s="52"/>
       <c r="J34" s="38" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="K34" s="63">
         <v>43502</v>
@@ -12162,7 +12023,7 @@
         <v>375</v>
       </c>
       <c r="B35" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C35" s="62">
         <v>3</v>
@@ -12182,7 +12043,7 @@
       <c r="H35" s="52"/>
       <c r="I35" s="52"/>
       <c r="J35" s="38" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="K35" s="63">
         <v>43502</v>
@@ -12228,7 +12089,7 @@
         <v>375</v>
       </c>
       <c r="B36" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C36" s="62">
         <v>3</v>
@@ -12248,7 +12109,7 @@
       <c r="H36" s="52"/>
       <c r="I36" s="52"/>
       <c r="J36" s="38" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="K36" s="63">
         <v>43502</v>
@@ -12294,7 +12155,7 @@
         <v>375</v>
       </c>
       <c r="B37" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C37" s="62">
         <v>3</v>
@@ -12314,7 +12175,7 @@
       <c r="H37" s="52"/>
       <c r="I37" s="52"/>
       <c r="J37" s="38" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="K37" s="63">
         <v>43502</v>
@@ -12358,7 +12219,7 @@
         <v>375</v>
       </c>
       <c r="B38" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C38" s="62">
         <v>3</v>
@@ -12378,7 +12239,7 @@
       <c r="H38" s="52"/>
       <c r="I38" s="52"/>
       <c r="J38" s="38" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="K38" s="63">
         <v>43502</v>
@@ -12422,7 +12283,7 @@
         <v>375</v>
       </c>
       <c r="B39" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C39" s="62">
         <v>3</v>
@@ -12442,7 +12303,7 @@
       <c r="H39" s="52"/>
       <c r="I39" s="52"/>
       <c r="J39" s="38" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="K39" s="63">
         <v>43502</v>
@@ -12490,7 +12351,7 @@
         <v>375</v>
       </c>
       <c r="B40" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C40" s="62">
         <v>3</v>
@@ -12510,7 +12371,7 @@
       <c r="H40" s="52"/>
       <c r="I40" s="52"/>
       <c r="J40" s="38" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="K40" s="63">
         <v>43502</v>
@@ -12556,7 +12417,7 @@
         <v>375</v>
       </c>
       <c r="B41" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C41" s="62">
         <v>3</v>
@@ -12576,7 +12437,7 @@
       <c r="H41" s="52"/>
       <c r="I41" s="52"/>
       <c r="J41" s="38" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="K41" s="63">
         <v>43502</v>
@@ -12620,7 +12481,7 @@
         <v>375</v>
       </c>
       <c r="B42" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C42" s="62">
         <v>3</v>
@@ -12640,7 +12501,7 @@
       <c r="H42" s="52"/>
       <c r="I42" s="52"/>
       <c r="J42" s="38" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="K42" s="63">
         <v>43502</v>
@@ -12690,7 +12551,7 @@
         <v>375</v>
       </c>
       <c r="B43" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C43" s="62">
         <v>3</v>
@@ -12710,7 +12571,7 @@
       <c r="H43" s="52"/>
       <c r="I43" s="52"/>
       <c r="J43" s="38" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="K43" s="63">
         <v>43502</v>
@@ -12762,7 +12623,7 @@
         <v>375</v>
       </c>
       <c r="B44" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C44" s="62">
         <v>3</v>
@@ -12782,7 +12643,7 @@
       <c r="H44" s="52"/>
       <c r="I44" s="52"/>
       <c r="J44" s="38" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="K44" s="63">
         <v>43502</v>
@@ -12832,7 +12693,7 @@
         <v>375</v>
       </c>
       <c r="B45" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C45" s="62">
         <v>3</v>
@@ -12852,7 +12713,7 @@
       <c r="H45" s="52"/>
       <c r="I45" s="52"/>
       <c r="J45" s="38" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="K45" s="63">
         <v>43502</v>
@@ -12898,7 +12759,7 @@
         <v>375</v>
       </c>
       <c r="B46" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C46" s="62">
         <v>3</v>
@@ -12918,7 +12779,7 @@
       <c r="H46" s="52"/>
       <c r="I46" s="52"/>
       <c r="J46" s="38" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="K46" s="63">
         <v>43502</v>
@@ -12964,7 +12825,7 @@
         <v>375</v>
       </c>
       <c r="B47" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C47" s="62">
         <v>3</v>
@@ -12984,7 +12845,7 @@
       <c r="H47" s="52"/>
       <c r="I47" s="52"/>
       <c r="J47" s="38" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="K47" s="63">
         <v>43502</v>
@@ -13028,7 +12889,7 @@
         <v>375</v>
       </c>
       <c r="B48" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C48" s="62">
         <v>3</v>
@@ -13048,7 +12909,7 @@
       <c r="H48" s="52"/>
       <c r="I48" s="52"/>
       <c r="J48" s="38" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="K48" s="63">
         <v>43502</v>
@@ -13094,7 +12955,7 @@
         <v>375</v>
       </c>
       <c r="B49" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C49" s="62">
         <v>3</v>
@@ -13114,7 +12975,7 @@
       <c r="H49" s="52"/>
       <c r="I49" s="52"/>
       <c r="J49" s="38" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="K49" s="63">
         <v>43502</v>
@@ -13162,7 +13023,7 @@
         <v>375</v>
       </c>
       <c r="B50" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C50" s="62">
         <v>3</v>
@@ -13182,7 +13043,7 @@
       <c r="H50" s="52"/>
       <c r="I50" s="52"/>
       <c r="J50" s="38" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="K50" s="63">
         <v>43502</v>
@@ -13232,7 +13093,7 @@
         <v>375</v>
       </c>
       <c r="B51" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C51" s="62">
         <v>3</v>
@@ -13252,7 +13113,7 @@
       <c r="H51" s="52"/>
       <c r="I51" s="52"/>
       <c r="J51" s="38" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="K51" s="63">
         <v>43502</v>
@@ -13298,7 +13159,7 @@
         <v>375</v>
       </c>
       <c r="B52" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C52" s="62">
         <v>3</v>
@@ -13318,7 +13179,7 @@
       <c r="H52" s="52"/>
       <c r="I52" s="52"/>
       <c r="J52" s="38" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="K52" s="63">
         <v>43502</v>
@@ -13362,7 +13223,7 @@
         <v>375</v>
       </c>
       <c r="B53" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C53" s="62">
         <v>3</v>
@@ -13382,7 +13243,7 @@
       <c r="H53" s="52"/>
       <c r="I53" s="52"/>
       <c r="J53" s="38" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="K53" s="63">
         <v>43502</v>
@@ -13428,7 +13289,7 @@
         <v>375</v>
       </c>
       <c r="B54" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C54" s="62">
         <v>3</v>
@@ -13448,7 +13309,7 @@
       <c r="H54" s="52"/>
       <c r="I54" s="52"/>
       <c r="J54" s="38" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="K54" s="63">
         <v>43502</v>
@@ -13492,7 +13353,7 @@
         <v>375</v>
       </c>
       <c r="B55" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C55" s="62">
         <v>3</v>
@@ -13512,7 +13373,7 @@
       <c r="H55" s="52"/>
       <c r="I55" s="52"/>
       <c r="J55" s="38" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="K55" s="63">
         <v>43502</v>
@@ -13562,7 +13423,7 @@
         <v>375</v>
       </c>
       <c r="B56" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C56" s="62">
         <v>3</v>
@@ -13582,7 +13443,7 @@
       <c r="H56" s="52"/>
       <c r="I56" s="52"/>
       <c r="J56" s="38" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="K56" s="63">
         <v>43502</v>
@@ -13628,7 +13489,7 @@
         <v>375</v>
       </c>
       <c r="B57" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C57" s="62">
         <v>3</v>
@@ -13648,7 +13509,7 @@
       <c r="H57" s="52"/>
       <c r="I57" s="52"/>
       <c r="J57" s="38" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="K57" s="63">
         <v>43502</v>
@@ -13700,7 +13561,7 @@
         <v>375</v>
       </c>
       <c r="B58" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C58" s="62">
         <v>3</v>
@@ -13720,7 +13581,7 @@
       <c r="H58" s="52"/>
       <c r="I58" s="52"/>
       <c r="J58" s="38" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="K58" s="63">
         <v>43502</v>
@@ -13768,7 +13629,7 @@
         <v>375</v>
       </c>
       <c r="B59" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C59" s="62">
         <v>3</v>
@@ -13788,7 +13649,7 @@
       <c r="H59" s="52"/>
       <c r="I59" s="52"/>
       <c r="J59" s="38" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="K59" s="63">
         <v>43502</v>
@@ -13832,7 +13693,7 @@
         <v>375</v>
       </c>
       <c r="B60" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C60" s="62">
         <v>3</v>
@@ -13852,7 +13713,7 @@
       <c r="H60" s="52"/>
       <c r="I60" s="52"/>
       <c r="J60" s="38" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="K60" s="63">
         <v>43502</v>
@@ -13898,7 +13759,7 @@
         <v>375</v>
       </c>
       <c r="B61" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C61" s="62">
         <v>3</v>
@@ -13918,7 +13779,7 @@
       <c r="H61" s="52"/>
       <c r="I61" s="52"/>
       <c r="J61" s="38" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="K61" s="63">
         <v>43502</v>
@@ -13962,7 +13823,7 @@
         <v>375</v>
       </c>
       <c r="B62" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C62" s="62">
         <v>3</v>
@@ -13982,7 +13843,7 @@
       <c r="H62" s="52"/>
       <c r="I62" s="52"/>
       <c r="J62" s="38" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="K62" s="63">
         <v>43502</v>
@@ -14030,7 +13891,7 @@
         <v>375</v>
       </c>
       <c r="B63" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C63" s="62">
         <v>3</v>
@@ -14050,7 +13911,7 @@
       <c r="H63" s="52"/>
       <c r="I63" s="52"/>
       <c r="J63" s="38" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="K63" s="63">
         <v>43502</v>
@@ -14100,7 +13961,7 @@
         <v>375</v>
       </c>
       <c r="B64" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C64" s="62">
         <v>3</v>
@@ -14120,7 +13981,7 @@
       <c r="H64" s="52"/>
       <c r="I64" s="52"/>
       <c r="J64" s="38" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="K64" s="63">
         <v>43502</v>
@@ -14168,7 +14029,7 @@
         <v>375</v>
       </c>
       <c r="B65" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C65" s="62">
         <v>3</v>
@@ -14188,7 +14049,7 @@
       <c r="H65" s="52"/>
       <c r="I65" s="52"/>
       <c r="J65" s="38" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="K65" s="63">
         <v>43502</v>
@@ -14240,7 +14101,7 @@
         <v>375</v>
       </c>
       <c r="B66" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C66" s="62">
         <v>3</v>
@@ -14260,7 +14121,7 @@
       <c r="H66" s="52"/>
       <c r="I66" s="52"/>
       <c r="J66" s="38" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="K66" s="63">
         <v>43502</v>
@@ -14304,7 +14165,7 @@
         <v>375</v>
       </c>
       <c r="B67" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C67" s="62">
         <v>3</v>
@@ -14324,7 +14185,7 @@
       <c r="H67" s="52"/>
       <c r="I67" s="52"/>
       <c r="J67" s="38" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="K67" s="63">
         <v>43502</v>
@@ -14370,7 +14231,7 @@
         <v>375</v>
       </c>
       <c r="B68" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C68" s="62">
         <v>3</v>
@@ -14390,7 +14251,7 @@
       <c r="H68" s="52"/>
       <c r="I68" s="52"/>
       <c r="J68" s="38" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="K68" s="63">
         <v>43502</v>
@@ -14440,7 +14301,7 @@
         <v>375</v>
       </c>
       <c r="B69" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C69" s="62">
         <v>3</v>
@@ -14460,7 +14321,7 @@
       <c r="H69" s="52"/>
       <c r="I69" s="52"/>
       <c r="J69" s="38" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="K69" s="63">
         <v>43502</v>
@@ -14504,7 +14365,7 @@
         <v>375</v>
       </c>
       <c r="B70" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C70" s="62">
         <v>3</v>
@@ -14524,7 +14385,7 @@
       <c r="H70" s="52"/>
       <c r="I70" s="52"/>
       <c r="J70" s="38" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="K70" s="63">
         <v>43502</v>
@@ -14572,7 +14433,7 @@
         <v>375</v>
       </c>
       <c r="B71" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C71" s="62">
         <v>3</v>
@@ -14592,7 +14453,7 @@
       <c r="H71" s="52"/>
       <c r="I71" s="52"/>
       <c r="J71" s="38" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="K71" s="63">
         <v>43502</v>
@@ -14638,7 +14499,7 @@
         <v>375</v>
       </c>
       <c r="B72" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C72" s="62">
         <v>3</v>
@@ -14658,7 +14519,7 @@
       <c r="H72" s="52"/>
       <c r="I72" s="52"/>
       <c r="J72" s="38" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="K72" s="63">
         <v>43502</v>
@@ -14710,7 +14571,7 @@
         <v>375</v>
       </c>
       <c r="B73" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C73" s="62">
         <v>3</v>
@@ -14730,7 +14591,7 @@
       <c r="H73" s="52"/>
       <c r="I73" s="52"/>
       <c r="J73" s="38" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="K73" s="63">
         <v>43502</v>
@@ -14774,7 +14635,7 @@
         <v>375</v>
       </c>
       <c r="B74" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C74" s="62">
         <v>3</v>
@@ -14794,7 +14655,7 @@
       <c r="H74" s="52"/>
       <c r="I74" s="52"/>
       <c r="J74" s="38" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="K74" s="63">
         <v>43502</v>
@@ -14838,7 +14699,7 @@
         <v>375</v>
       </c>
       <c r="B75" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C75" s="62">
         <v>3</v>
@@ -14858,7 +14719,7 @@
       <c r="H75" s="52"/>
       <c r="I75" s="52"/>
       <c r="J75" s="38" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="K75" s="63">
         <v>43502</v>
@@ -14908,7 +14769,7 @@
         <v>375</v>
       </c>
       <c r="B76" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C76" s="62">
         <v>3</v>
@@ -14928,7 +14789,7 @@
       <c r="H76" s="52"/>
       <c r="I76" s="52"/>
       <c r="J76" s="38" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="K76" s="63">
         <v>43502</v>
@@ -14972,7 +14833,7 @@
         <v>375</v>
       </c>
       <c r="B77" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C77" s="62">
         <v>3</v>
@@ -14992,7 +14853,7 @@
       <c r="H77" s="52"/>
       <c r="I77" s="52"/>
       <c r="J77" s="38" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="K77" s="63">
         <v>43502</v>
@@ -15038,7 +14899,7 @@
         <v>375</v>
       </c>
       <c r="B78" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C78" s="62">
         <v>3</v>
@@ -15058,7 +14919,7 @@
       <c r="H78" s="52"/>
       <c r="I78" s="52"/>
       <c r="J78" s="38" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="K78" s="63">
         <v>43502</v>
@@ -15104,7 +14965,7 @@
         <v>375</v>
       </c>
       <c r="B79" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C79" s="62">
         <v>3</v>
@@ -15124,7 +14985,7 @@
       <c r="H79" s="52"/>
       <c r="I79" s="52"/>
       <c r="J79" s="38" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="K79" s="63">
         <v>43502</v>
@@ -15172,7 +15033,7 @@
         <v>375</v>
       </c>
       <c r="B80" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C80" s="62">
         <v>3</v>
@@ -15192,7 +15053,7 @@
       <c r="H80" s="52"/>
       <c r="I80" s="52"/>
       <c r="J80" s="38" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="K80" s="63">
         <v>43502</v>
@@ -15238,7 +15099,7 @@
         <v>375</v>
       </c>
       <c r="B81" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C81" s="62">
         <v>3</v>
@@ -15258,7 +15119,7 @@
       <c r="H81" s="52"/>
       <c r="I81" s="52"/>
       <c r="J81" s="38" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="K81" s="63">
         <v>43502</v>
@@ -15304,7 +15165,7 @@
         <v>375</v>
       </c>
       <c r="B82" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C82" s="62">
         <v>3</v>
@@ -15324,7 +15185,7 @@
       <c r="H82" s="52"/>
       <c r="I82" s="52"/>
       <c r="J82" s="38" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="K82" s="63">
         <v>43502</v>
@@ -15370,7 +15231,7 @@
         <v>375</v>
       </c>
       <c r="B83" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C83" s="62">
         <v>3</v>
@@ -15390,7 +15251,7 @@
       <c r="H83" s="52"/>
       <c r="I83" s="52"/>
       <c r="J83" s="38" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="K83" s="63">
         <v>43502</v>
@@ -15436,7 +15297,7 @@
         <v>375</v>
       </c>
       <c r="B84" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C84" s="62">
         <v>3</v>
@@ -15456,7 +15317,7 @@
       <c r="H84" s="52"/>
       <c r="I84" s="52"/>
       <c r="J84" s="38" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="K84" s="63">
         <v>43502</v>
@@ -15502,7 +15363,7 @@
         <v>375</v>
       </c>
       <c r="B85" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C85" s="62">
         <v>3</v>
@@ -15522,7 +15383,7 @@
       <c r="H85" s="52"/>
       <c r="I85" s="52"/>
       <c r="J85" s="38" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="K85" s="63">
         <v>43502</v>
@@ -15566,7 +15427,7 @@
         <v>375</v>
       </c>
       <c r="B86" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C86" s="62">
         <v>2</v>
@@ -15586,7 +15447,7 @@
       <c r="H86" s="52"/>
       <c r="I86" s="52"/>
       <c r="J86" s="38" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="K86" s="63">
         <v>43517</v>
@@ -15640,7 +15501,7 @@
         <v>375</v>
       </c>
       <c r="B87" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C87" s="62">
         <v>2</v>
@@ -15660,7 +15521,7 @@
       <c r="H87" s="52"/>
       <c r="I87" s="52"/>
       <c r="J87" s="38" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K87" s="63">
         <v>43517</v>
@@ -15712,7 +15573,7 @@
         <v>375</v>
       </c>
       <c r="B88" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C88" s="62">
         <v>2</v>
@@ -15732,7 +15593,7 @@
       <c r="H88" s="52"/>
       <c r="I88" s="52"/>
       <c r="J88" s="38" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="K88" s="63">
         <v>43517</v>
@@ -15780,7 +15641,7 @@
         <v>375</v>
       </c>
       <c r="B89" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C89" s="62">
         <v>2</v>
@@ -15800,7 +15661,7 @@
       <c r="H89" s="52"/>
       <c r="I89" s="52"/>
       <c r="J89" s="38" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="K89" s="63">
         <v>43517</v>
@@ -15844,7 +15705,7 @@
         <v>375</v>
       </c>
       <c r="B90" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C90" s="62">
         <v>2</v>
@@ -15864,7 +15725,7 @@
       <c r="H90" s="52"/>
       <c r="I90" s="52"/>
       <c r="J90" s="38" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="K90" s="63">
         <v>43517</v>
@@ -15908,7 +15769,7 @@
         <v>375</v>
       </c>
       <c r="B91" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C91" s="62">
         <v>2</v>
@@ -15928,7 +15789,7 @@
       <c r="H91" s="52"/>
       <c r="I91" s="52"/>
       <c r="J91" s="38" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="K91" s="63">
         <v>43517</v>
@@ -15978,7 +15839,7 @@
         <v>375</v>
       </c>
       <c r="B92" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C92" s="62">
         <v>2</v>
@@ -15998,7 +15859,7 @@
       <c r="H92" s="52"/>
       <c r="I92" s="52"/>
       <c r="J92" s="38" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="K92" s="63">
         <v>43517</v>
@@ -16050,7 +15911,7 @@
         <v>375</v>
       </c>
       <c r="B93" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C93" s="62">
         <v>2</v>
@@ -16070,7 +15931,7 @@
       <c r="H93" s="52"/>
       <c r="I93" s="52"/>
       <c r="J93" s="38" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="K93" s="63">
         <v>43517</v>
@@ -16116,7 +15977,7 @@
         <v>375</v>
       </c>
       <c r="B94" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C94" s="62">
         <v>2</v>
@@ -16136,7 +15997,7 @@
       <c r="H94" s="52"/>
       <c r="I94" s="52"/>
       <c r="J94" s="38" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="K94" s="63">
         <v>43517</v>
@@ -16180,7 +16041,7 @@
         <v>375</v>
       </c>
       <c r="B95" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C95" s="62">
         <v>2</v>
@@ -16200,7 +16061,7 @@
       <c r="H95" s="52"/>
       <c r="I95" s="52"/>
       <c r="J95" s="38" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="K95" s="63">
         <v>43517</v>
@@ -16248,7 +16109,7 @@
         <v>375</v>
       </c>
       <c r="B96" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C96" s="62">
         <v>2</v>
@@ -16268,7 +16129,7 @@
       <c r="H96" s="52"/>
       <c r="I96" s="52"/>
       <c r="J96" s="38" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="K96" s="63">
         <v>43517</v>
@@ -16322,7 +16183,7 @@
         <v>375</v>
       </c>
       <c r="B97" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C97" s="62">
         <v>2</v>
@@ -16342,7 +16203,7 @@
       <c r="H97" s="52"/>
       <c r="I97" s="52"/>
       <c r="J97" s="38" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="K97" s="63">
         <v>43517</v>
@@ -16388,7 +16249,7 @@
         <v>375</v>
       </c>
       <c r="B98" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C98" s="62">
         <v>2</v>
@@ -16408,7 +16269,7 @@
       <c r="H98" s="52"/>
       <c r="I98" s="52"/>
       <c r="J98" s="38" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="K98" s="63">
         <v>43517</v>
@@ -16452,7 +16313,7 @@
         <v>375</v>
       </c>
       <c r="B99" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C99" s="62">
         <v>2</v>
@@ -16472,7 +16333,7 @@
       <c r="H99" s="52"/>
       <c r="I99" s="52"/>
       <c r="J99" s="38" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="K99" s="63">
         <v>43517</v>
@@ -16514,7 +16375,7 @@
         <v>375</v>
       </c>
       <c r="B100" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C100" s="62">
         <v>2</v>
@@ -16534,7 +16395,7 @@
       <c r="H100" s="52"/>
       <c r="I100" s="52"/>
       <c r="J100" s="38" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="K100" s="63">
         <v>43517</v>
@@ -16580,7 +16441,7 @@
         <v>375</v>
       </c>
       <c r="B101" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C101" s="62">
         <v>5</v>
@@ -16600,7 +16461,7 @@
       <c r="H101" s="52"/>
       <c r="I101" s="52"/>
       <c r="J101" s="38" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="K101" s="63">
         <v>43523</v>
@@ -16646,7 +16507,7 @@
         <v>375</v>
       </c>
       <c r="B102" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C102" s="62">
         <v>5</v>
@@ -16666,7 +16527,7 @@
       <c r="H102" s="52"/>
       <c r="I102" s="52"/>
       <c r="J102" s="38" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="K102" s="63">
         <v>43523</v>
@@ -16712,7 +16573,7 @@
         <v>375</v>
       </c>
       <c r="B103" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C103" s="62">
         <v>5</v>
@@ -16732,7 +16593,7 @@
       <c r="H103" s="52"/>
       <c r="I103" s="52"/>
       <c r="J103" s="38" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="K103" s="63">
         <v>43523</v>
@@ -16776,7 +16637,7 @@
         <v>375</v>
       </c>
       <c r="B104" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C104" s="62">
         <v>5</v>
@@ -16796,7 +16657,7 @@
       <c r="H104" s="52"/>
       <c r="I104" s="52"/>
       <c r="J104" s="38" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="K104" s="63">
         <v>43523</v>
@@ -16844,7 +16705,7 @@
         <v>375</v>
       </c>
       <c r="B105" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C105" s="62">
         <v>5</v>
@@ -16864,7 +16725,7 @@
       <c r="H105" s="52"/>
       <c r="I105" s="52"/>
       <c r="J105" s="38" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="K105" s="63">
         <v>43523</v>
@@ -16910,7 +16771,7 @@
         <v>375</v>
       </c>
       <c r="B106" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C106" s="62">
         <v>5</v>
@@ -16930,7 +16791,7 @@
       <c r="H106" s="52"/>
       <c r="I106" s="52"/>
       <c r="J106" s="38" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="K106" s="63">
         <v>43523</v>
@@ -16976,7 +16837,7 @@
         <v>375</v>
       </c>
       <c r="B107" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C107" s="62">
         <v>5</v>
@@ -16996,7 +16857,7 @@
       <c r="H107" s="52"/>
       <c r="I107" s="52"/>
       <c r="J107" s="38" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="K107" s="63">
         <v>43523</v>
@@ -17047,7 +16908,7 @@
         <v>375</v>
       </c>
       <c r="B108" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C108" s="62">
         <v>5</v>
@@ -17067,7 +16928,7 @@
       <c r="H108" s="52"/>
       <c r="I108" s="52"/>
       <c r="J108" s="38" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="K108" s="63">
         <v>43523</v>
@@ -17118,7 +16979,7 @@
         <v>375</v>
       </c>
       <c r="B109" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C109" s="62">
         <v>5</v>
@@ -17138,7 +16999,7 @@
       <c r="H109" s="52"/>
       <c r="I109" s="52"/>
       <c r="J109" s="38" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="K109" s="63">
         <v>43523</v>
@@ -17174,7 +17035,7 @@
         <v>375</v>
       </c>
       <c r="B110" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C110" s="62">
         <v>5</v>
@@ -17194,7 +17055,7 @@
       <c r="H110" s="52"/>
       <c r="I110" s="52"/>
       <c r="J110" s="38" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="K110" s="63">
         <v>43523</v>
@@ -17238,7 +17099,7 @@
         <v>375</v>
       </c>
       <c r="B111" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C111" s="62">
         <v>5</v>
@@ -17258,7 +17119,7 @@
       <c r="H111" s="52"/>
       <c r="I111" s="52"/>
       <c r="J111" s="38" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="K111" s="63">
         <v>43523</v>
@@ -17306,7 +17167,7 @@
         <v>375</v>
       </c>
       <c r="B112" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C112" s="62">
         <v>5</v>
@@ -17326,7 +17187,7 @@
       <c r="H112" s="52"/>
       <c r="I112" s="52"/>
       <c r="J112" s="38" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="K112" s="63">
         <v>43523</v>
@@ -17370,7 +17231,7 @@
         <v>375</v>
       </c>
       <c r="B113" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C113" s="62">
         <v>5</v>
@@ -17390,7 +17251,7 @@
       <c r="H113" s="52"/>
       <c r="I113" s="52"/>
       <c r="J113" s="38" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="K113" s="63">
         <v>43523</v>
@@ -17434,7 +17295,7 @@
         <v>375</v>
       </c>
       <c r="B114" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C114" s="62">
         <v>5</v>
@@ -17454,7 +17315,7 @@
       <c r="H114" s="52"/>
       <c r="I114" s="52"/>
       <c r="J114" s="38" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="K114" s="63">
         <v>43523</v>
@@ -17500,7 +17361,7 @@
         <v>375</v>
       </c>
       <c r="B115" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C115" s="62">
         <v>5</v>
@@ -17520,7 +17381,7 @@
       <c r="H115" s="52"/>
       <c r="I115" s="52"/>
       <c r="J115" s="38" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="K115" s="63">
         <v>43523</v>
@@ -17566,7 +17427,7 @@
         <v>375</v>
       </c>
       <c r="B116" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C116" s="62">
         <v>6</v>
@@ -17586,7 +17447,7 @@
       <c r="H116" s="52"/>
       <c r="I116" s="52"/>
       <c r="J116" s="38" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="K116" s="63">
         <v>43523</v>
@@ -17632,7 +17493,7 @@
         <v>375</v>
       </c>
       <c r="B117" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C117" s="62">
         <v>6</v>
@@ -17652,7 +17513,7 @@
       <c r="H117" s="52"/>
       <c r="I117" s="52"/>
       <c r="J117" s="38" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="K117" s="63">
         <v>43523</v>
@@ -17700,7 +17561,7 @@
         <v>375</v>
       </c>
       <c r="B118" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C118" s="62">
         <v>6</v>
@@ -17720,7 +17581,7 @@
       <c r="H118" s="52"/>
       <c r="I118" s="52"/>
       <c r="J118" s="38" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="K118" s="63">
         <v>43523</v>
@@ -17764,7 +17625,7 @@
         <v>375</v>
       </c>
       <c r="B119" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C119" s="62">
         <v>6</v>
@@ -17784,7 +17645,7 @@
       <c r="H119" s="52"/>
       <c r="I119" s="52"/>
       <c r="J119" s="38" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="K119" s="63">
         <v>43523</v>
@@ -17832,7 +17693,7 @@
         <v>375</v>
       </c>
       <c r="B120" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C120" s="62">
         <v>6</v>
@@ -17852,7 +17713,7 @@
       <c r="H120" s="52"/>
       <c r="I120" s="52"/>
       <c r="J120" s="38" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="K120" s="63">
         <v>43523</v>
@@ -17918,7 +17779,7 @@
       <c r="H121" s="52"/>
       <c r="I121" s="52"/>
       <c r="J121" s="38" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="K121" s="63">
         <v>43524</v>
@@ -17978,7 +17839,7 @@
       <c r="H122" s="52"/>
       <c r="I122" s="52"/>
       <c r="J122" s="38" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="K122" s="63">
         <v>43524</v>
@@ -18050,7 +17911,7 @@
       <c r="H123" s="52"/>
       <c r="I123" s="52"/>
       <c r="J123" s="38" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="K123" s="63">
         <v>43524</v>
@@ -18118,7 +17979,7 @@
       <c r="H124" s="52"/>
       <c r="I124" s="52"/>
       <c r="J124" s="38" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K124" s="63">
         <v>43524</v>
@@ -18186,7 +18047,7 @@
       <c r="H125" s="52"/>
       <c r="I125" s="52"/>
       <c r="J125" s="38" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="K125" s="63">
         <v>43524</v>
@@ -18250,7 +18111,7 @@
       <c r="H126" s="52"/>
       <c r="I126" s="52"/>
       <c r="J126" s="38" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="K126" s="63">
         <v>43524</v>
@@ -18311,7 +18172,7 @@
       <c r="H127" s="52"/>
       <c r="I127" s="52"/>
       <c r="J127" s="38" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="K127" s="63">
         <v>43524</v>
@@ -24339,7 +24200,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B2" s="63">
         <v>43523</v>
@@ -24349,13 +24210,13 @@
       </c>
       <c r="D2" s="38"/>
       <c r="E2" s="40" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="F2" s="38" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="G2" s="76" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="H2" s="57" t="s">
         <v>226</v>
@@ -24368,7 +24229,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B3" s="63">
         <v>43523</v>
@@ -24378,13 +24239,13 @@
       </c>
       <c r="D3" s="38"/>
       <c r="E3" s="40" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F3" s="38" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="G3" s="77" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="H3" s="57" t="s">
         <v>226</v>
@@ -24397,7 +24258,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="38" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B4" s="63">
         <v>43523</v>
@@ -24407,13 +24268,13 @@
       </c>
       <c r="D4" s="38"/>
       <c r="E4" s="40" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="F4" s="38" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="G4" s="76" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="H4" s="57" t="s">
         <v>226</v>
@@ -25848,7 +25709,7 @@
       <c r="I2" s="19"/>
       <c r="J2" s="19"/>
       <c r="K2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L2" s="80"/>
       <c r="M2" s="80"/>
@@ -25895,7 +25756,7 @@
       <c r="I3" s="19"/>
       <c r="J3" s="19"/>
       <c r="K3" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L3" s="80"/>
       <c r="M3" s="80"/>
@@ -25936,7 +25797,7 @@
       <c r="I4" s="19"/>
       <c r="J4" s="19"/>
       <c r="K4" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L4" s="80"/>
       <c r="M4" s="80"/>
@@ -25977,7 +25838,7 @@
       <c r="I5" s="19"/>
       <c r="J5" s="19"/>
       <c r="K5" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L5" s="80"/>
       <c r="M5" s="80"/>
@@ -26018,7 +25879,7 @@
       <c r="I6" s="19"/>
       <c r="J6" s="19"/>
       <c r="K6" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L6" s="80"/>
       <c r="M6" s="80"/>
@@ -26059,7 +25920,7 @@
       <c r="I7" s="19"/>
       <c r="J7" s="19"/>
       <c r="K7" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L7" s="80"/>
       <c r="M7" s="80"/>
@@ -26100,7 +25961,7 @@
       <c r="I8" s="19"/>
       <c r="J8" s="19"/>
       <c r="K8" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L8" s="80"/>
       <c r="M8" s="80"/>
@@ -26143,7 +26004,7 @@
       <c r="I9" s="19"/>
       <c r="J9" s="19"/>
       <c r="K9" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="L9" s="80"/>
       <c r="M9" s="80">
@@ -26186,7 +26047,7 @@
       <c r="I10" s="19"/>
       <c r="J10" s="19"/>
       <c r="K10" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L10" s="80"/>
       <c r="M10" s="80"/>
@@ -26227,7 +26088,7 @@
       <c r="I11" s="19"/>
       <c r="J11" s="19"/>
       <c r="K11" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L11" s="80"/>
       <c r="M11" s="80"/>
@@ -26270,7 +26131,7 @@
       <c r="I12" s="19"/>
       <c r="J12" s="19"/>
       <c r="K12" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L12" s="80"/>
       <c r="M12" s="80"/>
@@ -26313,7 +26174,7 @@
       <c r="I13" s="19"/>
       <c r="J13" s="19"/>
       <c r="K13" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L13" s="80"/>
       <c r="M13" s="80"/>
@@ -26354,7 +26215,7 @@
       <c r="I14" s="19"/>
       <c r="J14" s="19"/>
       <c r="K14" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="L14" s="80"/>
       <c r="M14" s="80"/>
@@ -26395,7 +26256,7 @@
       <c r="I15" s="19"/>
       <c r="J15" s="19"/>
       <c r="K15" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L15" s="80"/>
       <c r="M15" s="80"/>
@@ -26436,7 +26297,7 @@
       <c r="I16" s="19"/>
       <c r="J16" s="19"/>
       <c r="K16" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L16" s="80"/>
       <c r="M16" s="80"/>
@@ -26479,7 +26340,7 @@
       <c r="I17" s="19"/>
       <c r="J17" s="19"/>
       <c r="K17" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L17" s="80"/>
       <c r="M17" s="80"/>
@@ -26520,7 +26381,7 @@
       <c r="I18" s="19"/>
       <c r="J18" s="19"/>
       <c r="K18" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L18" s="80"/>
       <c r="M18" s="80"/>
@@ -26563,7 +26424,7 @@
       <c r="I19" s="19"/>
       <c r="J19" s="19"/>
       <c r="K19" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L19" s="80"/>
       <c r="M19" s="80"/>
@@ -26604,7 +26465,7 @@
       <c r="I20" s="19"/>
       <c r="J20" s="19"/>
       <c r="K20" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L20" s="80"/>
       <c r="M20" s="80"/>
@@ -26647,7 +26508,7 @@
       <c r="I21" s="19"/>
       <c r="J21" s="19"/>
       <c r="K21" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L21" s="80"/>
       <c r="M21" s="80"/>
@@ -26688,7 +26549,7 @@
       <c r="I22" s="19"/>
       <c r="J22" s="19"/>
       <c r="K22" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L22" s="80"/>
       <c r="M22" s="80"/>
@@ -26729,7 +26590,7 @@
       <c r="I23" s="19"/>
       <c r="J23" s="19"/>
       <c r="K23" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L23" s="80"/>
       <c r="M23" s="80"/>
@@ -26772,7 +26633,7 @@
       <c r="I24" s="19"/>
       <c r="J24" s="19"/>
       <c r="K24" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L24" s="80"/>
       <c r="M24" s="80"/>
@@ -26813,7 +26674,7 @@
       <c r="I25" s="19"/>
       <c r="J25" s="19"/>
       <c r="K25" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L25" s="80"/>
       <c r="M25" s="80"/>
@@ -26854,7 +26715,7 @@
       <c r="I26" s="19"/>
       <c r="J26" s="19"/>
       <c r="K26" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L26" s="80"/>
       <c r="M26" s="80"/>
@@ -26897,7 +26758,7 @@
       <c r="I27" s="19"/>
       <c r="J27" s="19"/>
       <c r="K27" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L27" s="80"/>
       <c r="M27" s="80"/>
@@ -26938,7 +26799,7 @@
       <c r="I28" s="19"/>
       <c r="J28" s="19"/>
       <c r="K28" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L28" s="80"/>
       <c r="M28" s="80"/>
@@ -26979,7 +26840,7 @@
       <c r="I29" s="19"/>
       <c r="J29" s="19"/>
       <c r="K29" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L29" s="80"/>
       <c r="M29" s="80"/>
@@ -27020,7 +26881,7 @@
       <c r="I30" s="19"/>
       <c r="J30" s="19"/>
       <c r="K30" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L30" s="80"/>
       <c r="M30" s="80"/>
@@ -27063,7 +26924,7 @@
       <c r="I31" s="19"/>
       <c r="J31" s="19"/>
       <c r="K31" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L31" s="80"/>
       <c r="M31" s="80"/>
@@ -27106,7 +26967,7 @@
       <c r="I32" s="19"/>
       <c r="J32" s="19"/>
       <c r="K32" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L32" s="80"/>
       <c r="M32" s="80"/>
@@ -27149,7 +27010,7 @@
       <c r="I33" s="19"/>
       <c r="J33" s="19"/>
       <c r="K33" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L33" s="80"/>
       <c r="M33" s="80"/>
@@ -27192,7 +27053,7 @@
       <c r="I34" s="19"/>
       <c r="J34" s="19"/>
       <c r="K34" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L34" s="80"/>
       <c r="M34" s="80"/>
@@ -27235,7 +27096,7 @@
       <c r="I35" s="19"/>
       <c r="J35" s="19"/>
       <c r="K35" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L35" s="80"/>
       <c r="M35" s="80"/>
@@ -27276,7 +27137,7 @@
       <c r="I36" s="19"/>
       <c r="J36" s="19"/>
       <c r="K36" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L36" s="80"/>
       <c r="M36" s="80"/>
@@ -27319,7 +27180,7 @@
       <c r="I37" s="19"/>
       <c r="J37" s="19"/>
       <c r="K37" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L37" s="80"/>
       <c r="M37" s="80"/>
@@ -27360,7 +27221,7 @@
       <c r="I38" s="19"/>
       <c r="J38" s="19"/>
       <c r="K38" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L38" s="80"/>
       <c r="M38" s="80"/>
@@ -27401,7 +27262,7 @@
       <c r="I39" s="19"/>
       <c r="J39" s="19"/>
       <c r="K39" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L39" s="80"/>
       <c r="M39" s="80"/>
@@ -27442,7 +27303,7 @@
       <c r="I40" s="19"/>
       <c r="J40" s="19"/>
       <c r="K40" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L40" s="80"/>
       <c r="M40" s="80"/>
@@ -27485,7 +27346,7 @@
       <c r="I41" s="19"/>
       <c r="J41" s="19"/>
       <c r="K41" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L41" s="80"/>
       <c r="M41" s="80"/>
@@ -27528,7 +27389,7 @@
       <c r="I42" s="19"/>
       <c r="J42" s="19"/>
       <c r="K42" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L42" s="80"/>
       <c r="M42" s="80"/>
@@ -27569,7 +27430,7 @@
       <c r="I43" s="19"/>
       <c r="J43" s="19"/>
       <c r="K43" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L43" s="80"/>
       <c r="M43" s="80"/>
@@ -27610,7 +27471,7 @@
       <c r="I44" s="19"/>
       <c r="J44" s="19"/>
       <c r="K44" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L44" s="80"/>
       <c r="M44" s="80"/>
@@ -27651,7 +27512,7 @@
       <c r="I45" s="19"/>
       <c r="J45" s="19"/>
       <c r="K45" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L45" s="80"/>
       <c r="M45" s="80"/>
@@ -27692,7 +27553,7 @@
       <c r="I46" s="19"/>
       <c r="J46" s="19"/>
       <c r="K46" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L46" s="80"/>
       <c r="M46" s="80"/>
@@ -27733,7 +27594,7 @@
       <c r="I47" s="19"/>
       <c r="J47" s="19"/>
       <c r="K47" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L47" s="80"/>
       <c r="M47" s="80"/>
@@ -27774,7 +27635,7 @@
       <c r="I48" s="19"/>
       <c r="J48" s="19"/>
       <c r="K48" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L48" s="80"/>
       <c r="M48" s="80"/>
@@ -27815,7 +27676,7 @@
       <c r="I49" s="19"/>
       <c r="J49" s="19"/>
       <c r="K49" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L49" s="80"/>
       <c r="M49" s="80"/>
@@ -27856,7 +27717,7 @@
       <c r="I50" s="19"/>
       <c r="J50" s="19"/>
       <c r="K50" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L50" s="80"/>
       <c r="M50" s="80"/>
@@ -27897,7 +27758,7 @@
       <c r="I51" s="19"/>
       <c r="J51" s="19"/>
       <c r="K51" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L51" s="80"/>
       <c r="M51" s="80"/>
@@ -27940,7 +27801,7 @@
       <c r="I52" s="19"/>
       <c r="J52" s="19"/>
       <c r="K52" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L52" s="80"/>
       <c r="M52" s="80"/>
@@ -27981,7 +27842,7 @@
       <c r="I53" s="19"/>
       <c r="J53" s="19"/>
       <c r="K53" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L53" s="80"/>
       <c r="M53" s="80"/>
@@ -28022,7 +27883,7 @@
       <c r="I54" s="19"/>
       <c r="J54" s="19"/>
       <c r="K54" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L54" s="80"/>
       <c r="M54" s="80"/>
@@ -28063,7 +27924,7 @@
       <c r="I55" s="19"/>
       <c r="J55" s="19"/>
       <c r="K55" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="L55" s="80"/>
       <c r="M55" s="80"/>
@@ -28104,7 +27965,7 @@
       <c r="I56" s="19"/>
       <c r="J56" s="19"/>
       <c r="K56" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="L56" s="80"/>
       <c r="M56" s="80"/>
@@ -28145,7 +28006,7 @@
       <c r="I57" s="19"/>
       <c r="J57" s="19"/>
       <c r="K57" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="L57" s="80"/>
       <c r="M57" s="80"/>
@@ -28186,7 +28047,7 @@
       <c r="I58" s="19"/>
       <c r="J58" s="19"/>
       <c r="K58" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="L58" s="80"/>
       <c r="M58" s="80"/>
@@ -28227,7 +28088,7 @@
       <c r="I59" s="19"/>
       <c r="J59" s="19"/>
       <c r="K59" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="L59" s="80"/>
       <c r="M59" s="80"/>
@@ -28268,7 +28129,7 @@
       <c r="I60" s="19"/>
       <c r="J60" s="19"/>
       <c r="K60" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L60" s="80"/>
       <c r="M60" s="80"/>
@@ -28309,7 +28170,7 @@
       <c r="I61" s="19"/>
       <c r="J61" s="19"/>
       <c r="K61" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="L61" s="80"/>
       <c r="M61" s="80"/>
@@ -28350,7 +28211,7 @@
       <c r="I62" s="19"/>
       <c r="J62" s="19"/>
       <c r="K62" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L62" s="80"/>
       <c r="M62" s="80"/>
@@ -28391,7 +28252,7 @@
       <c r="I63" s="19"/>
       <c r="J63" s="19"/>
       <c r="K63" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="L63" s="80"/>
       <c r="M63" s="80"/>
@@ -28432,7 +28293,7 @@
       <c r="I64" s="19"/>
       <c r="J64" s="19"/>
       <c r="K64" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L64" s="80"/>
       <c r="M64" s="80"/>
@@ -28473,7 +28334,7 @@
       <c r="I65" s="19"/>
       <c r="J65" s="19"/>
       <c r="K65" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="L65" s="80"/>
       <c r="M65" s="80"/>
@@ -28514,7 +28375,7 @@
       <c r="I66" s="19"/>
       <c r="J66" s="19"/>
       <c r="K66" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="L66" s="80"/>
       <c r="M66" s="80"/>
@@ -28555,7 +28416,7 @@
       <c r="I67" s="19"/>
       <c r="J67" s="19"/>
       <c r="K67" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="L67" s="80"/>
       <c r="M67" s="80"/>
@@ -28596,7 +28457,7 @@
       <c r="I68" s="19"/>
       <c r="J68" s="19"/>
       <c r="K68" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="L68" s="80"/>
       <c r="M68" s="80"/>
@@ -28637,7 +28498,7 @@
       <c r="I69" s="19"/>
       <c r="J69" s="19"/>
       <c r="K69" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="L69" s="80"/>
       <c r="M69" s="80"/>
@@ -28678,7 +28539,7 @@
       <c r="I70" s="19"/>
       <c r="J70" s="19"/>
       <c r="K70" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="L70" s="80"/>
       <c r="M70" s="80"/>
@@ -28719,7 +28580,7 @@
       <c r="I71" s="19"/>
       <c r="J71" s="19"/>
       <c r="K71" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="L71" s="80">
         <v>6</v>
@@ -28760,7 +28621,7 @@
       <c r="I72" s="19"/>
       <c r="J72" s="19"/>
       <c r="K72" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L72" s="80"/>
       <c r="M72" s="80"/>
@@ -28801,7 +28662,7 @@
       <c r="I73" s="19"/>
       <c r="J73" s="19"/>
       <c r="K73" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="L73" s="80"/>
       <c r="M73" s="80"/>
@@ -28842,7 +28703,7 @@
       <c r="I74" s="19"/>
       <c r="J74" s="19"/>
       <c r="K74" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L74" s="80"/>
       <c r="M74" s="80"/>
@@ -28885,7 +28746,7 @@
       <c r="I75" s="19"/>
       <c r="J75" s="19"/>
       <c r="K75" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L75" s="80"/>
       <c r="M75" s="80"/>
@@ -28926,7 +28787,7 @@
       <c r="I76" s="19"/>
       <c r="J76" s="19"/>
       <c r="K76" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L76" s="80"/>
       <c r="M76" s="80"/>
@@ -28967,7 +28828,7 @@
       <c r="I77" s="19"/>
       <c r="J77" s="19"/>
       <c r="K77" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L77" s="80"/>
       <c r="M77" s="80"/>
@@ -29008,7 +28869,7 @@
       <c r="I78" s="19"/>
       <c r="J78" s="19"/>
       <c r="K78" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L78" s="80"/>
       <c r="M78" s="80"/>
@@ -29049,7 +28910,7 @@
       <c r="I79" s="19"/>
       <c r="J79" s="19"/>
       <c r="K79" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L79" s="80"/>
       <c r="M79" s="80"/>
@@ -29090,7 +28951,7 @@
       <c r="I80" s="19"/>
       <c r="J80" s="19"/>
       <c r="K80" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L80" s="80"/>
       <c r="M80" s="80"/>
@@ -29131,7 +28992,7 @@
       <c r="I81" s="19"/>
       <c r="J81" s="19"/>
       <c r="K81" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L81" s="80"/>
       <c r="M81" s="80">
@@ -29174,7 +29035,7 @@
       <c r="I82" s="19"/>
       <c r="J82" s="19"/>
       <c r="K82" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="L82" s="80"/>
       <c r="M82" s="80"/>
@@ -29215,7 +29076,7 @@
       <c r="I83" s="19"/>
       <c r="J83" s="19"/>
       <c r="K83" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="L83" s="80"/>
       <c r="M83" s="80"/>
@@ -29256,7 +29117,7 @@
       <c r="I84" s="19"/>
       <c r="J84" s="19"/>
       <c r="K84" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="L84" s="80"/>
       <c r="M84" s="80"/>
@@ -29297,7 +29158,7 @@
       <c r="I85" s="19"/>
       <c r="J85" s="19"/>
       <c r="K85" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="L85" s="80"/>
       <c r="M85" s="80"/>
@@ -29338,7 +29199,7 @@
       <c r="I86" s="19"/>
       <c r="J86" s="19"/>
       <c r="K86" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="L86" s="80"/>
       <c r="M86" s="80"/>
@@ -29379,7 +29240,7 @@
       <c r="I87" s="19"/>
       <c r="J87" s="19"/>
       <c r="K87" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="L87" s="80"/>
       <c r="M87" s="80"/>
@@ -29420,7 +29281,7 @@
       <c r="I88" s="19"/>
       <c r="J88" s="19"/>
       <c r="K88" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="L88" s="80"/>
       <c r="M88" s="80"/>
@@ -29461,7 +29322,7 @@
       <c r="I89" s="19"/>
       <c r="J89" s="19"/>
       <c r="K89" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="L89" s="80"/>
       <c r="M89" s="80"/>
@@ -29502,7 +29363,7 @@
       <c r="I90" s="19"/>
       <c r="J90" s="19"/>
       <c r="K90" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="L90" s="74"/>
       <c r="M90" s="74"/>
@@ -29543,7 +29404,7 @@
       <c r="I91" s="19"/>
       <c r="J91" s="19"/>
       <c r="K91" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="L91" s="74"/>
       <c r="M91" s="74"/>
@@ -29584,7 +29445,7 @@
       <c r="I92" s="19"/>
       <c r="J92" s="19"/>
       <c r="K92" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="L92" s="74"/>
       <c r="M92" s="74"/>
@@ -29625,7 +29486,7 @@
       <c r="I93" s="19"/>
       <c r="J93" s="19"/>
       <c r="K93" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="L93" s="74"/>
       <c r="M93" s="74">
@@ -29668,7 +29529,7 @@
       <c r="I94" s="19"/>
       <c r="J94" s="19"/>
       <c r="K94" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="L94" s="74"/>
       <c r="M94" s="74">
@@ -29711,7 +29572,7 @@
       <c r="I95" s="19"/>
       <c r="J95" s="19"/>
       <c r="K95" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="L95" s="74"/>
       <c r="M95" s="74"/>
@@ -29752,7 +29613,7 @@
       <c r="I96" s="19"/>
       <c r="J96" s="19"/>
       <c r="K96" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L96" s="74"/>
       <c r="M96" s="74"/>
@@ -29793,7 +29654,7 @@
       <c r="I97" s="19"/>
       <c r="J97" s="19"/>
       <c r="K97" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L97" s="74"/>
       <c r="M97" s="74"/>
@@ -29834,7 +29695,7 @@
       <c r="I98" s="19"/>
       <c r="J98" s="19"/>
       <c r="K98" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="L98" s="74"/>
       <c r="M98" s="74"/>
@@ -29875,7 +29736,7 @@
       <c r="I99" s="19"/>
       <c r="J99" s="19"/>
       <c r="K99" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="L99" s="74"/>
       <c r="M99" s="74"/>
@@ -29916,7 +29777,7 @@
       <c r="I100" s="19"/>
       <c r="J100" s="19"/>
       <c r="K100" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="L100" s="74"/>
       <c r="M100" s="74"/>
@@ -29953,7 +29814,7 @@
         <v>36</v>
       </c>
       <c r="K101" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="L101" s="74"/>
       <c r="M101" s="74"/>
@@ -29989,7 +29850,7 @@
         <v>36</v>
       </c>
       <c r="K102" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="L102" s="74"/>
       <c r="M102" s="74"/>

</xml_diff>